<commit_message>
Versión antes de aplicar el crossover de la lecture 3
</commit_message>
<xml_diff>
--- a/Lab 4/Assignment 4 comparison.xlsx
+++ b/Lab 4/Assignment 4 comparison.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D911F52F-6D7A-7A4E-B857-8A14F647858F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1FCE94-FAA4-964D-950D-4DBDF5ECB365}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>algorithm name</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>F10 mean</t>
+  </si>
+  <si>
+    <t>DE</t>
   </si>
 </sst>
 </file>
@@ -671,12 +674,13 @@
   <dimension ref="B1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -752,24 +756,38 @@
     </row>
     <row r="4" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C4" s="4">
-        <v>121742.7625</v>
+        <v>80501.269499999995</v>
       </c>
       <c r="D4" s="2">
-        <v>180287.98499999999</v>
+        <v>958286.59499999997</v>
       </c>
       <c r="E4" s="2">
-        <v>3236033850</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
+        <v>1493601325</v>
+      </c>
+      <c r="F4" s="2">
+        <v>114310.7055</v>
+      </c>
+      <c r="G4" s="2">
+        <v>38134.527000000002</v>
+      </c>
+      <c r="H4" s="2">
+        <v>51408609500</v>
+      </c>
+      <c r="I4" s="2">
+        <v>3310.82555</v>
+      </c>
+      <c r="J4" s="2">
+        <v>21.128739499999998</v>
+      </c>
+      <c r="K4" s="2">
+        <v>470.67778499999997</v>
+      </c>
+      <c r="L4" s="2">
+        <v>758.30847500000004</v>
+      </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
@@ -777,43 +795,43 @@
       </c>
       <c r="C6" s="4">
         <f>MAX(C3:C4)</f>
-        <v>121742.7625</v>
+        <v>80501.269499999995</v>
       </c>
       <c r="D6" s="4">
         <f t="shared" ref="D6:L6" si="0">MAX(D3:D4)</f>
-        <v>180287.98499999999</v>
+        <v>958286.59499999997</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>3236033850</v>
+        <v>1493601325</v>
       </c>
       <c r="F6" s="4">
         <f t="shared" si="0"/>
-        <v>272</v>
+        <v>114310.7055</v>
       </c>
       <c r="G6" s="4">
         <f t="shared" si="0"/>
-        <v>136</v>
+        <v>38134.527000000002</v>
       </c>
       <c r="H6" s="4">
         <f t="shared" si="0"/>
-        <v>31.8</v>
+        <v>51408609500</v>
       </c>
       <c r="I6" s="4">
         <f t="shared" si="0"/>
-        <v>5.3199999999999997E-2</v>
+        <v>3310.82555</v>
       </c>
       <c r="J6" s="4">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>21.128739499999998</v>
       </c>
       <c r="K6" s="4">
         <f t="shared" si="0"/>
-        <v>12.2</v>
+        <v>470.67778499999997</v>
       </c>
       <c r="L6" s="4">
         <f t="shared" si="0"/>
-        <v>147</v>
+        <v>758.30847500000004</v>
       </c>
     </row>
     <row r="7" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -865,43 +883,43 @@
       </c>
       <c r="D9" s="5">
         <f t="shared" ref="D9:L10" si="1">IF(D$6=0,0,D3/D$6)</f>
-        <v>1.8803249700749609E-4</v>
+        <v>3.5375638328740268E-5</v>
       </c>
       <c r="E9" s="5">
         <f t="shared" si="1"/>
-        <v>1.9808198236245275E-3</v>
+        <v>4.2916405420301831E-3</v>
       </c>
       <c r="F9" s="5">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2.3794796717443059E-3</v>
       </c>
       <c r="G9" s="5">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3.5663219318283401E-3</v>
       </c>
       <c r="H9" s="5">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>6.18573431751738E-10</v>
       </c>
       <c r="I9" s="5">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.6068499894233327E-5</v>
       </c>
       <c r="J9" s="5">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.99390690107187896</v>
       </c>
       <c r="K9" s="5">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2.5920067589338215E-2</v>
       </c>
       <c r="L9" s="5">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.19385250837398327</v>
       </c>
       <c r="M9" s="5">
         <f>SUM(C9:L9)</f>
-        <v>7.002168852320632</v>
+        <v>1.2239683639375998</v>
       </c>
     </row>
     <row r="10" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -922,35 +940,35 @@
       </c>
       <c r="F10" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10" s="5">
         <f>SUM(C10:L10)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -965,7 +983,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="A2" sqref="A2:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1004,237 +1022,684 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
-        <v>83112500000</v>
+        <v>67923210000</v>
       </c>
       <c r="B2" s="4">
-        <v>164373300000</v>
+        <v>105783300000</v>
       </c>
       <c r="C2" s="4">
-        <v>1978593000000000</v>
+        <v>1781265000000000</v>
+      </c>
+      <c r="D2" s="4">
+        <v>135666200000</v>
+      </c>
+      <c r="E2" s="4">
+        <v>38593470000</v>
+      </c>
+      <c r="F2" s="4">
+        <v>4.489044E+16</v>
+      </c>
+      <c r="G2" s="4">
+        <v>3407259000</v>
+      </c>
+      <c r="H2" s="4">
+        <v>21125470</v>
+      </c>
+      <c r="I2" s="4">
+        <v>386125800</v>
+      </c>
+      <c r="J2" s="4">
+        <v>687723200</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
-        <v>114486100000</v>
+        <v>79170560000</v>
       </c>
       <c r="B3" s="4">
-        <v>196875600000</v>
+        <v>97323860000</v>
       </c>
       <c r="C3" s="4">
-        <v>2396823000000000</v>
+        <v>1573398000000000</v>
+      </c>
+      <c r="D3" s="4">
+        <v>136289600000</v>
+      </c>
+      <c r="E3" s="4">
+        <v>28633720000</v>
+      </c>
+      <c r="F3" s="4">
+        <v>6.699683E+16</v>
+      </c>
+      <c r="G3" s="4">
+        <v>3507623000</v>
+      </c>
+      <c r="H3" s="4">
+        <v>21229310</v>
+      </c>
+      <c r="I3" s="4">
+        <v>487545700</v>
+      </c>
+      <c r="J3" s="4">
+        <v>770658000</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
-        <v>149496100000</v>
+        <v>74183740000</v>
       </c>
       <c r="B4" s="4">
-        <v>71288920000</v>
+        <v>90045750000</v>
       </c>
       <c r="C4" s="4">
-        <v>5249154000000000</v>
+        <v>1068987000000000</v>
+      </c>
+      <c r="D4" s="4">
+        <v>145475500000</v>
+      </c>
+      <c r="E4" s="4">
+        <v>39884030000</v>
+      </c>
+      <c r="F4" s="4">
+        <v>4.597023E+16</v>
+      </c>
+      <c r="G4" s="4">
+        <v>3191990000</v>
+      </c>
+      <c r="H4" s="4">
+        <v>20977280</v>
+      </c>
+      <c r="I4" s="4">
+        <v>504693300</v>
+      </c>
+      <c r="J4" s="4">
+        <v>730727600</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
-        <v>102005200000</v>
+        <v>90705870000</v>
       </c>
       <c r="B5" s="4">
-        <v>161674800000</v>
+        <v>107190900000</v>
       </c>
       <c r="C5" s="4">
-        <v>5309538000000000</v>
+        <v>1647230000000000</v>
+      </c>
+      <c r="D5" s="4">
+        <v>117950700000</v>
+      </c>
+      <c r="E5" s="4">
+        <v>37283010000</v>
+      </c>
+      <c r="F5" s="4">
+        <v>6.249443E+16</v>
+      </c>
+      <c r="G5" s="4">
+        <v>3137175000</v>
+      </c>
+      <c r="H5" s="4">
+        <v>21145180</v>
+      </c>
+      <c r="I5" s="4">
+        <v>513645400</v>
+      </c>
+      <c r="J5" s="4">
+        <v>785434100</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
-        <v>128063000000</v>
+        <v>86409130000</v>
       </c>
       <c r="B6" s="4">
-        <v>221217800000</v>
+        <v>103934300000</v>
       </c>
       <c r="C6" s="4">
-        <v>3033840000000000</v>
+        <v>1416933000000000</v>
+      </c>
+      <c r="D6" s="4">
+        <v>95979790000</v>
+      </c>
+      <c r="E6" s="4">
+        <v>42329010000</v>
+      </c>
+      <c r="F6" s="4">
+        <v>6.12361E+16</v>
+      </c>
+      <c r="G6" s="4">
+        <v>2779774000</v>
+      </c>
+      <c r="H6" s="4">
+        <v>21157070</v>
+      </c>
+      <c r="I6" s="4">
+        <v>488941000</v>
+      </c>
+      <c r="J6" s="4">
+        <v>883090600</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
-        <v>119120400000</v>
+        <v>78785120000</v>
       </c>
       <c r="B7" s="4">
-        <v>97768810000</v>
+        <v>94051690000</v>
       </c>
       <c r="C7" s="4">
-        <v>2677452000000000</v>
+        <v>1688509000000000</v>
+      </c>
+      <c r="D7" s="4">
+        <v>131347000000</v>
+      </c>
+      <c r="E7" s="4">
+        <v>33219950000</v>
+      </c>
+      <c r="F7" s="4">
+        <v>6.326047E+16</v>
+      </c>
+      <c r="G7" s="4">
+        <v>3771613000</v>
+      </c>
+      <c r="H7" s="4">
+        <v>21153610</v>
+      </c>
+      <c r="I7" s="4">
+        <v>438520600</v>
+      </c>
+      <c r="J7" s="4">
+        <v>732375300</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
-        <v>132689700000</v>
+        <v>68678010000</v>
       </c>
       <c r="B8" s="4">
-        <v>204986000000</v>
+        <v>67942280000</v>
       </c>
       <c r="C8" s="4">
-        <v>4240892000000000</v>
+        <v>1684294000000000</v>
+      </c>
+      <c r="D8" s="4">
+        <v>75206040000</v>
+      </c>
+      <c r="E8" s="4">
+        <v>39173190000</v>
+      </c>
+      <c r="F8" s="4">
+        <v>2.919928E+16</v>
+      </c>
+      <c r="G8" s="4">
+        <v>3379354000</v>
+      </c>
+      <c r="H8" s="4">
+        <v>20999680</v>
+      </c>
+      <c r="I8" s="4">
+        <v>518372700</v>
+      </c>
+      <c r="J8" s="4">
+        <v>716323600</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
-        <v>127096200000</v>
+        <v>79523310000</v>
       </c>
       <c r="B9" s="4">
-        <v>296291200000</v>
+        <v>113467300000</v>
       </c>
       <c r="C9" s="4">
-        <v>5633914000000000</v>
+        <v>1315186000000000</v>
+      </c>
+      <c r="D9" s="4">
+        <v>117517600000</v>
+      </c>
+      <c r="E9" s="4">
+        <v>42752220000</v>
+      </c>
+      <c r="F9" s="4">
+        <v>8.233069E+16</v>
+      </c>
+      <c r="G9" s="4">
+        <v>3545326000</v>
+      </c>
+      <c r="H9" s="4">
+        <v>21239680</v>
+      </c>
+      <c r="I9" s="4">
+        <v>463204400</v>
+      </c>
+      <c r="J9" s="4">
+        <v>804896400</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
-        <v>134853300000</v>
+        <v>72482060000</v>
       </c>
       <c r="B10" s="4">
-        <v>171776400000</v>
+        <v>66781060000</v>
       </c>
       <c r="C10" s="4">
-        <v>2798172000000000</v>
+        <v>1885020000000000</v>
+      </c>
+      <c r="D10" s="4">
+        <v>131450700000</v>
+      </c>
+      <c r="E10" s="4">
+        <v>38417300000</v>
+      </c>
+      <c r="F10" s="4">
+        <v>4.689085E+16</v>
+      </c>
+      <c r="G10" s="4">
+        <v>3039341000</v>
+      </c>
+      <c r="H10" s="4">
+        <v>21123310</v>
+      </c>
+      <c r="I10" s="4">
+        <v>434853200</v>
+      </c>
+      <c r="J10" s="4">
+        <v>621198100</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
-        <v>115502700000</v>
+        <v>80314760000</v>
       </c>
       <c r="B11" s="4">
-        <v>235458900000</v>
+        <v>90830880000</v>
       </c>
       <c r="C11" s="4">
-        <v>2678478000000000</v>
+        <v>989423700000000</v>
+      </c>
+      <c r="D11" s="4">
+        <v>100053700000</v>
+      </c>
+      <c r="E11" s="4">
+        <v>41646840000</v>
+      </c>
+      <c r="F11" s="4">
+        <v>4.201291E+16</v>
+      </c>
+      <c r="G11" s="4">
+        <v>3442875000</v>
+      </c>
+      <c r="H11" s="4">
+        <v>21156360</v>
+      </c>
+      <c r="I11" s="4">
+        <v>449134900</v>
+      </c>
+      <c r="J11" s="4">
+        <v>831096700</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
-        <v>125823600000</v>
+        <v>56426660000</v>
       </c>
       <c r="B12" s="4">
-        <v>89528770000</v>
+        <v>90897390000</v>
       </c>
       <c r="C12" s="4">
-        <v>2199134000000000</v>
+        <v>1592365000000000</v>
+      </c>
+      <c r="D12" s="4">
+        <v>98572030000</v>
+      </c>
+      <c r="E12" s="4">
+        <v>37295120000</v>
+      </c>
+      <c r="F12" s="4">
+        <v>3.822761E+16</v>
+      </c>
+      <c r="G12" s="4">
+        <v>3440532000</v>
+      </c>
+      <c r="H12" s="4">
+        <v>21165280</v>
+      </c>
+      <c r="I12" s="4">
+        <v>477545100</v>
+      </c>
+      <c r="J12" s="4">
+        <v>809970900</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
-        <v>140128400000</v>
+        <v>95982760000</v>
       </c>
       <c r="B13" s="4">
-        <v>283813900000</v>
+        <v>109057400000</v>
       </c>
       <c r="C13" s="4">
-        <v>1776486000000000</v>
+        <v>1136752000000000</v>
+      </c>
+      <c r="D13" s="4">
+        <v>75314290000</v>
+      </c>
+      <c r="E13" s="4">
+        <v>38856520000</v>
+      </c>
+      <c r="F13" s="4">
+        <v>2.939014E+16</v>
+      </c>
+      <c r="G13" s="4">
+        <v>2629716000</v>
+      </c>
+      <c r="H13" s="4">
+        <v>21067850</v>
+      </c>
+      <c r="I13" s="4">
+        <v>424454200</v>
+      </c>
+      <c r="J13" s="4">
+        <v>752204300</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
-        <v>139561000000</v>
+        <v>75021880000</v>
       </c>
       <c r="B14" s="4">
-        <v>119580300000</v>
+        <v>92215610000</v>
       </c>
       <c r="C14" s="4">
-        <v>2419781000000000</v>
+        <v>1922128000000000</v>
+      </c>
+      <c r="D14" s="4">
+        <v>124575500000</v>
+      </c>
+      <c r="E14" s="4">
+        <v>35834210000</v>
+      </c>
+      <c r="F14" s="4">
+        <v>4.307598E+16</v>
+      </c>
+      <c r="G14" s="4">
+        <v>2958782000</v>
+      </c>
+      <c r="H14" s="4">
+        <v>21146580</v>
+      </c>
+      <c r="I14" s="4">
+        <v>473325000</v>
+      </c>
+      <c r="J14" s="4">
+        <v>694924500</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
-        <v>152942300000</v>
+        <v>89418930000</v>
       </c>
       <c r="B15" s="4">
-        <v>163919600000</v>
+        <v>98386800000</v>
       </c>
       <c r="C15" s="4">
-        <v>1683962000000000</v>
+        <v>1994117000000000</v>
+      </c>
+      <c r="D15" s="4">
+        <v>137707900000</v>
+      </c>
+      <c r="E15" s="4">
+        <v>39300840000</v>
+      </c>
+      <c r="F15" s="4">
+        <v>4.787641E+16</v>
+      </c>
+      <c r="G15" s="4">
+        <v>2850027000</v>
+      </c>
+      <c r="H15" s="4">
+        <v>21158060</v>
+      </c>
+      <c r="I15" s="4">
+        <v>499668200</v>
+      </c>
+      <c r="J15" s="4">
+        <v>757281300</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
-        <v>89275150000</v>
+        <v>66729390000</v>
       </c>
       <c r="B16" s="4">
-        <v>201392400000</v>
+        <v>116480300000</v>
       </c>
       <c r="C16" s="4">
-        <v>1885970000000000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1632864000000000</v>
+      </c>
+      <c r="D16" s="4">
+        <v>96434310000</v>
+      </c>
+      <c r="E16" s="4">
+        <v>33035270000</v>
+      </c>
+      <c r="F16" s="4">
+        <v>3.769899E+16</v>
+      </c>
+      <c r="G16" s="4">
+        <v>3345014000</v>
+      </c>
+      <c r="H16" s="4">
+        <v>21102260</v>
+      </c>
+      <c r="I16" s="4">
+        <v>500731100</v>
+      </c>
+      <c r="J16" s="4">
+        <v>775654800</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
-        <v>96725210000</v>
+        <v>71083850000</v>
       </c>
       <c r="B17" s="4">
-        <v>155145500000</v>
+        <v>102142100000</v>
       </c>
       <c r="C17" s="4">
-        <v>5532958000000000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1721994000000000</v>
+      </c>
+      <c r="D17" s="4">
+        <v>78681050000</v>
+      </c>
+      <c r="E17" s="4">
+        <v>40688440000</v>
+      </c>
+      <c r="F17" s="4">
+        <v>4.964775E+16</v>
+      </c>
+      <c r="G17" s="4">
+        <v>3683364000</v>
+      </c>
+      <c r="H17" s="4">
+        <v>21087400</v>
+      </c>
+      <c r="I17" s="4">
+        <v>487181700</v>
+      </c>
+      <c r="J17" s="4">
+        <v>715069000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
-        <v>95342690000</v>
+        <v>81350200000</v>
       </c>
       <c r="B18" s="4">
-        <v>261492100000</v>
+        <v>88269870000</v>
       </c>
       <c r="C18" s="4">
-        <v>6351786000000000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1415495000000000</v>
+      </c>
+      <c r="D18" s="4">
+        <v>127932800000</v>
+      </c>
+      <c r="E18" s="4">
+        <v>33757330000</v>
+      </c>
+      <c r="F18" s="4">
+        <v>5.583409E+16</v>
+      </c>
+      <c r="G18" s="4">
+        <v>3429200000</v>
+      </c>
+      <c r="H18" s="4">
+        <v>21178770</v>
+      </c>
+      <c r="I18" s="4">
+        <v>485860400</v>
+      </c>
+      <c r="J18" s="4">
+        <v>698167100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
-        <v>141957900000</v>
+        <v>59368390000</v>
       </c>
       <c r="B19" s="4">
-        <v>268771900000</v>
+        <v>100386100000</v>
       </c>
       <c r="C19" s="4">
-        <v>2495282000000000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>830615800000000</v>
+      </c>
+      <c r="D19" s="4">
+        <v>123089500000</v>
+      </c>
+      <c r="E19" s="4">
+        <v>43225190000</v>
+      </c>
+      <c r="F19" s="4">
+        <v>6.474646E+16</v>
+      </c>
+      <c r="G19" s="4">
+        <v>3887318000</v>
+      </c>
+      <c r="H19" s="4">
+        <v>21116450</v>
+      </c>
+      <c r="I19" s="4">
+        <v>500688500</v>
+      </c>
+      <c r="J19" s="4">
+        <v>784649500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
-        <v>125071100000</v>
+        <v>67207100000</v>
       </c>
       <c r="B20" s="4">
-        <v>136313400000</v>
+        <v>95003160000</v>
       </c>
       <c r="C20" s="4">
-        <v>2015110000000000</v>
-      </c>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1398926000000000</v>
+      </c>
+      <c r="D20" s="4">
+        <v>111449900000</v>
+      </c>
+      <c r="E20" s="4">
+        <v>43462710000</v>
+      </c>
+      <c r="F20" s="4">
+        <v>4.959444E+16</v>
+      </c>
+      <c r="G20" s="4">
+        <v>3289419000</v>
+      </c>
+      <c r="H20" s="4">
+        <v>21055210</v>
+      </c>
+      <c r="I20" s="4">
+        <v>390388100</v>
+      </c>
+      <c r="J20" s="4">
+        <v>825973800</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
-        <v>121602700000</v>
+        <v>66582900000</v>
       </c>
       <c r="B21" s="4">
-        <v>104090100000</v>
+        <v>86383140000</v>
       </c>
       <c r="C21" s="4">
-        <v>2363352000000000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1176524000000000</v>
+      </c>
+      <c r="D21" s="4">
+        <v>125520000000</v>
+      </c>
+      <c r="E21" s="4">
+        <v>35302170000</v>
+      </c>
+      <c r="F21" s="4">
+        <v>6.679809E+16</v>
+      </c>
+      <c r="G21" s="4">
+        <v>3500809000</v>
+      </c>
+      <c r="H21" s="4">
+        <v>21189980</v>
+      </c>
+      <c r="I21" s="4">
+        <v>488676400</v>
+      </c>
+      <c r="J21" s="4">
+        <v>788750700</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <f>SUM(A2:A21)/20</f>
-        <v>121742762500</v>
+        <v>75367391500</v>
       </c>
       <c r="B22" s="4">
         <f>SUM(B2:B21)/20</f>
-        <v>180287985000</v>
+        <v>95828659500</v>
       </c>
       <c r="C22" s="4">
         <f>SUM(C2:C21)/20</f>
-        <v>3236033850000000</v>
+        <v>1493601325000000</v>
+      </c>
+      <c r="D22" s="4">
+        <f t="shared" ref="D22:J22" si="0">SUM(D2:D21)/20</f>
+        <v>114310705500</v>
+      </c>
+      <c r="E22" s="4">
+        <f t="shared" si="0"/>
+        <v>38134527000</v>
+      </c>
+      <c r="F22" s="4">
+        <f t="shared" si="0"/>
+        <v>5.14086095E+16</v>
+      </c>
+      <c r="G22" s="4">
+        <f t="shared" si="0"/>
+        <v>3310825550</v>
+      </c>
+      <c r="H22" s="4">
+        <f t="shared" si="0"/>
+        <v>21128739.5</v>
+      </c>
+      <c r="I22" s="4">
+        <f t="shared" si="0"/>
+        <v>470677785</v>
+      </c>
+      <c r="J22" s="4">
+        <f t="shared" si="0"/>
+        <v>758308475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>